<commit_message>
Update Spreadsheets after Zayle, Shadow Cloak (patch 14.2)
</commit_message>
<xml_diff>
--- a/Spreadsheets/taunt_arena.xlsx
+++ b/Spreadsheets/taunt_arena.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="217">
   <si>
     <t>cost</t>
   </si>
@@ -52,13 +52,22 @@
     <t>Goldshire Footman</t>
   </si>
   <si>
+    <t>Shieldbearer</t>
+  </si>
+  <si>
+    <t>Witch's Apprentice</t>
+  </si>
+  <si>
     <t>Voidwalker</t>
   </si>
   <si>
-    <t>Witch's Apprentice</t>
-  </si>
-  <si>
-    <t>Shieldbearer</t>
+    <t>Twilight Geomancer</t>
+  </si>
+  <si>
+    <t>Public Defender</t>
+  </si>
+  <si>
+    <t>Dirty Rat</t>
   </si>
   <si>
     <t>Frostwolf Grunt</t>
@@ -67,168 +76,171 @@
     <t>Unstable Ghoul</t>
   </si>
   <si>
-    <t>Dirty Rat</t>
-  </si>
-  <si>
-    <t>Public Defender</t>
+    <t>Wickerflame Burnbristle</t>
   </si>
   <si>
     <t>Hired Gun</t>
   </si>
   <si>
-    <t>Wickerflame Burnbristle</t>
+    <t>Squirming Tentacle</t>
+  </si>
+  <si>
+    <t>Phantom Militia</t>
   </si>
   <si>
     <t>Deathlord</t>
   </si>
   <si>
+    <t>Ironfur Grizzly</t>
+  </si>
+  <si>
+    <t>Felguard</t>
+  </si>
+  <si>
+    <t>Silverback Patriarch</t>
+  </si>
+  <si>
     <t>Tauren Warrior</t>
   </si>
   <si>
-    <t>Phantom Militia</t>
-  </si>
-  <si>
-    <t>Silverback Patriarch</t>
-  </si>
-  <si>
-    <t>Ironfur Grizzly</t>
-  </si>
-  <si>
-    <t>Felguard</t>
-  </si>
-  <si>
-    <t>Squirming Tentacle</t>
+    <t>Sen'jin Shieldmasta</t>
+  </si>
+  <si>
+    <t>Infested Tauren</t>
+  </si>
+  <si>
+    <t>Faceless Shambler</t>
+  </si>
+  <si>
+    <t>Cyclopian Horror</t>
+  </si>
+  <si>
+    <t>Bloodhoof Brave</t>
+  </si>
+  <si>
+    <t>Totem Cruncher</t>
+  </si>
+  <si>
+    <t>Unpowered Steambot</t>
+  </si>
+  <si>
+    <t>Mogu'shan Warden</t>
+  </si>
+  <si>
+    <t>Hecklebot</t>
+  </si>
+  <si>
+    <t>Proud Defender</t>
   </si>
   <si>
     <t>Felsoul Inquisitor</t>
   </si>
   <si>
-    <t>Totem Cruncher</t>
-  </si>
-  <si>
-    <t>Unpowered Steambot</t>
-  </si>
-  <si>
-    <t>Infested Tauren</t>
-  </si>
-  <si>
-    <t>Faceless Shambler</t>
-  </si>
-  <si>
-    <t>Proud Defender</t>
-  </si>
-  <si>
-    <t>Bloodhoof Brave</t>
-  </si>
-  <si>
-    <t>Cyclopian Horror</t>
-  </si>
-  <si>
-    <t>Hecklebot</t>
-  </si>
-  <si>
-    <t>Sen'jin Shieldmasta</t>
-  </si>
-  <si>
     <t>Dread Corsair</t>
   </si>
   <si>
-    <t>Mogu'shan Warden</t>
+    <t>Alley Armorsmith</t>
+  </si>
+  <si>
+    <t>Second-Rate Bruiser</t>
+  </si>
+  <si>
+    <t>White Eyes</t>
+  </si>
+  <si>
+    <t>Booty Bay Bodyguard</t>
+  </si>
+  <si>
+    <t>Earth Elemental</t>
+  </si>
+  <si>
+    <t>Crazed Worshipper</t>
+  </si>
+  <si>
+    <t>Rotten Applebaum</t>
   </si>
   <si>
     <t>Witchwood Grizzly</t>
   </si>
   <si>
-    <t>Rotten Applebaum</t>
+    <t>Psych-o-Tron</t>
+  </si>
+  <si>
+    <t>Abomination</t>
+  </si>
+  <si>
+    <t>Convincing Infiltrator</t>
+  </si>
+  <si>
+    <t>Fen Creeper</t>
   </si>
   <si>
     <t>Bewitched Guardian</t>
   </si>
   <si>
-    <t>Booty Bay Bodyguard</t>
-  </si>
-  <si>
-    <t>Convincing Infiltrator</t>
-  </si>
-  <si>
     <t>Sludge Belcher</t>
   </si>
   <si>
-    <t>Second-Rate Bruiser</t>
-  </si>
-  <si>
-    <t>Alley Armorsmith</t>
-  </si>
-  <si>
-    <t>White Eyes</t>
-  </si>
-  <si>
-    <t>Earth Elemental</t>
-  </si>
-  <si>
-    <t>Fen Creeper</t>
-  </si>
-  <si>
-    <t>Psych-o-Tron</t>
-  </si>
-  <si>
-    <t>Abomination</t>
+    <t>Violet Warden</t>
+  </si>
+  <si>
+    <t>Safeguard</t>
+  </si>
+  <si>
+    <t>Aranasi Broodmother</t>
+  </si>
+  <si>
+    <t>Thing from Below</t>
+  </si>
+  <si>
+    <t>Wrathion</t>
+  </si>
+  <si>
+    <t>Jade Behemoth</t>
   </si>
   <si>
     <t>Ancient of Blossoms</t>
   </si>
   <si>
-    <t>Jade Behemoth</t>
-  </si>
-  <si>
-    <t>Wrathion</t>
-  </si>
-  <si>
-    <t>Aranasi Broodmother</t>
-  </si>
-  <si>
-    <t>Safeguard</t>
+    <t>Dark Arakkoa</t>
   </si>
   <si>
     <t>Lord of the Arena</t>
   </si>
   <si>
-    <t>Thing from Below</t>
+    <t>Sunwalker</t>
   </si>
   <si>
     <t>Hogger</t>
   </si>
   <si>
-    <t>Sunwalker</t>
-  </si>
-  <si>
-    <t>Violet Warden</t>
-  </si>
-  <si>
     <t>Tunnel Blaster</t>
   </si>
   <si>
+    <t>Twin Emperor Vek'lor</t>
+  </si>
+  <si>
+    <t>Bog Creeper</t>
+  </si>
+  <si>
     <t>Arch-Villain Rafaam</t>
   </si>
   <si>
-    <t>Bog Creeper</t>
+    <t>Furious Ettin</t>
   </si>
   <si>
     <t>Grimestreet Protector</t>
   </si>
   <si>
-    <t>Furious Ettin</t>
+    <t>Tirion Fordring</t>
+  </si>
+  <si>
+    <t>Al'Akir the Windlord</t>
   </si>
   <si>
     <t>Heroic Innkeeper</t>
   </si>
   <si>
-    <t>Tirion Fordring</t>
-  </si>
-  <si>
-    <t>Al'Akir the Windlord</t>
-  </si>
-  <si>
     <t>Ironbark Protector</t>
   </si>
   <si>
@@ -241,21 +253,21 @@
     <t>Basic</t>
   </si>
   <si>
+    <t>Classic</t>
+  </si>
+  <si>
     <t>The Witchwood</t>
   </si>
   <si>
-    <t>Classic</t>
+    <t>Whispers of the Old Gods</t>
+  </si>
+  <si>
+    <t>Mean Streets of Gadgetzan</t>
   </si>
   <si>
     <t>Naxxramas</t>
   </si>
   <si>
-    <t>Mean Streets of Gadgetzan</t>
-  </si>
-  <si>
-    <t>Whispers of the Old Gods</t>
-  </si>
-  <si>
     <t>Rise of Shadows</t>
   </si>
   <si>
@@ -277,33 +289,33 @@
     <t>Neutral</t>
   </si>
   <si>
+    <t>Shaman</t>
+  </si>
+  <si>
     <t>Warlock</t>
   </si>
   <si>
-    <t>Shaman</t>
-  </si>
-  <si>
     <t>Warrior</t>
   </si>
   <si>
     <t>Paladin</t>
   </si>
   <si>
+    <t>Priest</t>
+  </si>
+  <si>
     <t>Druid</t>
   </si>
   <si>
-    <t>Priest</t>
-  </si>
-  <si>
     <t>Minion</t>
   </si>
   <si>
+    <t>Beast</t>
+  </si>
+  <si>
     <t>Demon</t>
   </si>
   <si>
-    <t>Beast</t>
-  </si>
-  <si>
     <t>Mech</t>
   </si>
   <si>
@@ -319,123 +331,135 @@
     <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Add a random Shaman spell to your hand.</t>
   </si>
   <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Give your C'Thun\n&lt;b&gt;Taunt&lt;/b&gt; &lt;i&gt;(wherever it is).&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Your opponent\nsummons a random minion\nfrom their hand.</t>
+  </si>
+  <si>
     <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Deathrattle:&lt;/b&gt; Deal 1 damage to all minions.</t>
   </si>
   <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Your opponent\nsummons a random minion\nfrom their hand.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Divine Shield, Taunt, Lifesteal&lt;/b&gt;</t>
   </si>
   <si>
+    <t>&lt;b&gt;Echo&lt;/b&gt;\n&lt;b&gt;Taunt&lt;/b&gt;</t>
+  </si>
+  <si>
     <t>&lt;b&gt;Taunt. Deathrattle:&lt;/b&gt; Your opponent puts a minion from their deck into the battlefield.</t>
   </si>
   <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Destroy one of your Mana Crystals.</t>
+  </si>
+  <si>
     <t>&lt;b&gt;Taunt&lt;/b&gt;\nHas +3 Attack while damaged.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Echo&lt;/b&gt;\n&lt;b&gt;Taunt&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Destroy one of your Mana Crystals.</t>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Summon a 2/2 Slime.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Copy a friendly minion's Attack and Health.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Battlecry:&lt;/b&gt; Gain      +1 Health for each enemy minion.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Destroy your Totems. Gain +2/+2 for each destroyed.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Your opponent summons a minion from their deck.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\nHas +2 Attack while you [x]have no other minions.</t>
   </si>
   <si>
     <t>&lt;b&gt;Lifesteal&lt;/b&gt;\n&lt;b&gt;Taunt&lt;/b&gt;</t>
   </si>
   <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Destroy your Totems. Gain +2/+2 for each destroyed.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Summon a 2/2 Slime.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Copy a friendly minion's Attack and Health.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\nHas +2 Attack while you [x]have no other minions.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Battlecry:&lt;/b&gt; Gain      +1 Health for each enemy minion.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Your opponent summons a minion from their deck.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Taunt&lt;/b&gt;\nCosts (1) less per Attack of_your weapon.</t>
   </si>
   <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nWhenever this minion\ndeals damage, gain\nthat much Armor.</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nCosts (2) less if your\nopponent has at least\nthree minions.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Shuffle\n'The Storm Guardian' into your deck.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;&lt;b&gt;Overload&lt;/b&gt;:&lt;/b&gt; (3)</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt.&lt;/b&gt; Whenever this minion takes damage, give your C'Thun +1/+1 &lt;i&gt;(wherever it is).&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Restore #4 Health to your hero.</t>
+  </si>
+  <si>
     <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Lose 1 Health\nfor each card in your\nopponent's hand.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Restore #4 Health to your hero.</t>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Divine Shield&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Deathrattle:&lt;/b&gt; Deal 2\ndamage to ALL characters.</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;&lt;b&gt;Taunt&lt;/b&gt;&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Destroy a\n random enemy minion.</t>
   </si>
   <si>
     <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Gain +1 Health\n_for each card in your hand._</t>
   </si>
   <si>
-    <t>[x]&lt;b&gt;&lt;b&gt;Taunt&lt;/b&gt;&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Destroy a\n random enemy minion.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Taunt\nDeathrattle:&lt;/b&gt; Summon a 1/2 Slime with &lt;b&gt;Taunt&lt;/b&gt;.</t>
   </si>
   <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nCosts (2) less if your\nopponent has at least\nthree minions.</t>
-  </si>
-  <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nWhenever this minion\ndeals damage, gain\nthat much Armor.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Shuffle\n'The Storm Guardian' into your deck.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;&lt;b&gt;Overload&lt;/b&gt;:&lt;/b&gt; (3)</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Divine Shield&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Deathrattle:&lt;/b&gt; Deal 2\ndamage to ALL characters.</t>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Spell Damage +1&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Summon a 0/5\nVault Safe with &lt;b&gt;Taunt&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nWhen you draw this, restore\n#4 Health to your hero.</t>
+  </si>
+  <si>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nCosts (1) less for each\nTotem you've summoned\nthis game.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Battlecry:&lt;/b&gt; Draw cards until you draw one that isn't a Dragon.</t>
   </si>
   <si>
     <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Summon a{1}\n{0} &lt;b&gt;Jade Golem&lt;/b&gt;.@[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Summon a\n&lt;b&gt;Jade Golem&lt;/b&gt;.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;. &lt;b&gt;Battlecry:&lt;/b&gt; Draw cards until you draw one that isn't a Dragon.</t>
-  </si>
-  <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nWhen you draw this, restore\n4 Health to your hero.</t>
-  </si>
-  <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Summon a 0/5\nVault Safe with &lt;b&gt;Taunt&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\nCosts (1) less for each\nTotem you've summoned\nthis game.</t>
+    <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Give your C'Thun\n+3/+3 &lt;i&gt;(wherever it is).&lt;/i&gt;</t>
   </si>
   <si>
     <t>At the end of your turn, summon a 2/2 Gnoll with_&lt;b&gt;Taunt&lt;/b&gt;.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Spell Damage +1&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Deal 3 damage\nto all minions.</t>
   </si>
   <si>
+    <t>[x]&lt;b&gt;&lt;b&gt;Taunt&lt;/b&gt;\nBattlecry:&lt;/b&gt; If your C'Thun has\nat least 10 Attack, summon\nanother Emperor.</t>
+  </si>
+  <si>
     <t>&lt;b&gt;&lt;b&gt;Taunt&lt;/b&gt;\nBattlecry:&lt;/b&gt; Replace your hand and deck with &lt;b&gt;Legendary&lt;/b&gt; minions.</t>
   </si>
   <si>
     <t>[x]&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Battlecry:&lt;/b&gt; Give adjacent\n_minions &lt;b&gt;Divine Shield&lt;/b&gt;.</t>
   </si>
   <si>
+    <t>&lt;b&gt;&lt;b&gt;Divine Shield&lt;/b&gt;,&lt;/b&gt; &lt;b&gt;Taunt&lt;/b&gt; &lt;b&gt;Deathrattle:&lt;/b&gt; Equip a 5/3_Ashbringer.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Charge, Divine Shield, Taunt, Windfury&lt;/b&gt;</t>
+  </si>
+  <si>
     <t>&lt;b&gt;Taunt.&lt;/b&gt; &lt;b&gt;Battlecry:&lt;/b&gt; Gain +2/+2 for each other friendly minion.</t>
   </si>
   <si>
-    <t>&lt;b&gt;&lt;b&gt;Divine Shield&lt;/b&gt;,&lt;/b&gt; &lt;b&gt;Taunt&lt;/b&gt; &lt;b&gt;Deathrattle:&lt;/b&gt; Equip a 5/3_Ashbringer.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Charge, Divine Shield, Taunt, Windfury&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Taunt&lt;/b&gt;\n&lt;b&gt;Deathrattle:&lt;/b&gt; Go dormant. Restore 5 Health to awaken this minion.</t>
   </si>
   <si>
@@ -445,13 +469,22 @@
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS1_042.png</t>
   </si>
   <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_405.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_531.png</t>
+  </si>
+  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_065.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_531.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_405.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_284.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_300.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_790.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_121.png</t>
@@ -460,166 +493,169 @@
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/FP1_024.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_790.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_300.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_815.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_653.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_815.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_327.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_207.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/FP1_009.png</t>
   </si>
   <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_125.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_301.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_127.png</t>
+  </si>
+  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_390.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_207.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_127.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_125.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_301.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_327.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_179.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_249.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_174.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_337.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_218.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_583.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_809.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_396.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_058.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_551.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_527.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_583.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_809.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_249.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_174.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_551.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_218.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_337.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_058.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_179.png</t>
-  </si>
-  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/NEW1_022.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_396.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_756.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_652.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_324.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_187.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_250.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_321.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_667.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_623.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_667.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_145.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_097.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_039.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS1_069.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_507.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_187.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_039.png</t>
-  </si>
-  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/FP1_012.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_652.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_756.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_324.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_250.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS1_069.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_145.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_097.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_096.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_088.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_185.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_028.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_806.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_343.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_854.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_343.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_806.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_185.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_088.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_293.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_162.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_028.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_032.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/NEW1_040.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_032.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_096.png</t>
-  </si>
-  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_775.png</t>
   </si>
   <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_131.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_153.png</t>
+  </si>
+  <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_422.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/OG_153.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_120.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CFM_062.png</t>
   </si>
   <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/GIL_120.png</t>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_383.png</t>
+  </si>
+  <si>
+    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/NEW1_010.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/DAL_560.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/EX1_383.png</t>
-  </si>
-  <si>
-    <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/NEW1_010.png</t>
   </si>
   <si>
     <t>http://media.services.zam.com/v1/media/byName/hs/cards/enus/CS2_232.png</t>
@@ -999,7 +1035,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1048,16 +1084,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1066,10 +1102,10 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1080,31 +1116,28 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1115,19 +1148,19 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1136,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1150,28 +1183,31 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1182,28 +1218,28 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1214,28 +1250,28 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1246,16 +1282,16 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -1264,10 +1300,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1281,57 +1317,57 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1342,16 +1378,16 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -1360,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1374,28 +1410,28 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1406,28 +1442,28 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1438,16 +1474,16 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1456,10 +1492,10 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1470,31 +1506,28 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1505,19 +1538,19 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H16">
         <v>3</v>
@@ -1526,10 +1559,10 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1540,19 +1573,19 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -1561,10 +1594,10 @@
         <v>5</v>
       </c>
       <c r="J17" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1575,63 +1608,63 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>98</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1642,31 +1675,28 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J20" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1677,31 +1707,28 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1712,28 +1739,28 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1744,28 +1771,28 @@
         <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1776,16 +1803,16 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -1797,7 +1824,7 @@
         <v>112</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1808,28 +1835,31 @@
         <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G25" t="s">
+        <v>98</v>
       </c>
       <c r="H25">
         <v>2</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1840,28 +1870,31 @@
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G26" t="s">
+        <v>100</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J26" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1872,31 +1905,28 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J27" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1907,28 +1937,31 @@
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
+        <v>100</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="I28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1939,31 +1972,28 @@
         <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" t="s">
         <v>97</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1974,63 +2004,66 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G31" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="I31">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J31" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2041,28 +2074,28 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J32" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2073,28 +2106,28 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H33">
         <v>4</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J33" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2105,28 +2138,28 @@
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H34">
         <v>5</v>
       </c>
       <c r="I34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J34" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2137,28 +2170,28 @@
         <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
         <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2169,28 +2202,31 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G36" t="s">
+        <v>102</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I36">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J36" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2201,28 +2237,28 @@
         <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J37" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2233,28 +2269,28 @@
         <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J38" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2265,28 +2301,31 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F39" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="G39" t="s">
+        <v>98</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I39">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J39" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2297,31 +2336,31 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H40">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I40">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J40" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2332,28 +2371,28 @@
         <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J41" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2364,31 +2403,28 @@
         <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2399,92 +2435,92 @@
         <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F43" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J43" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F44" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H45">
         <v>3</v>
       </c>
       <c r="I45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J45" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2495,28 +2531,28 @@
         <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E46" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F46" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H46">
         <v>4</v>
       </c>
       <c r="I46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J46" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2527,31 +2563,31 @@
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G47" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H47">
         <v>4</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J47" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2562,31 +2598,31 @@
         <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E48" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G48" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H48">
         <v>4</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2597,28 +2633,28 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F49" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I49">
         <v>5</v>
       </c>
       <c r="J49" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2629,28 +2665,28 @@
         <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I50">
         <v>5</v>
       </c>
       <c r="J50" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2661,28 +2697,28 @@
         <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I51">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J51" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2693,28 +2729,28 @@
         <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I52">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J52" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2725,97 +2761,97 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E53" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F53" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53">
         <v>7</v>
       </c>
       <c r="J53" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D54" t="s">
         <v>85</v>
       </c>
       <c r="E54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I54">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J54" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F55" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H55">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I55">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J55" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
         <v>65</v>
@@ -2824,25 +2860,25 @@
         <v>79</v>
       </c>
       <c r="D56" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E56" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F56" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I56">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J56" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2853,28 +2889,28 @@
         <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E57" t="s">
         <v>90</v>
       </c>
       <c r="F57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I57">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J57" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2885,159 +2921,156 @@
         <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F58" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I58">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J58" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B59" t="s">
         <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F59" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I59">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J59" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B60" t="s">
         <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F60" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H60">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I60">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J60" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
         <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E61" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>93</v>
-      </c>
-      <c r="G61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H61">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I61">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J61" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
         <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E62" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F62" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H62">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I62">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J62" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3048,33 +3081,33 @@
         <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F63" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I63">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J63" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
         <v>73</v>
@@ -3083,25 +3116,156 @@
         <v>79</v>
       </c>
       <c r="D64" t="s">
+        <v>88</v>
+      </c>
+      <c r="E64" t="s">
+        <v>91</v>
+      </c>
+      <c r="F64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64">
+        <v>3</v>
+      </c>
+      <c r="I64">
+        <v>5</v>
+      </c>
+      <c r="J64" t="s">
+        <v>146</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
         <v>84</v>
       </c>
-      <c r="E64" t="s">
+      <c r="D65" t="s">
         <v>86</v>
       </c>
-      <c r="F64" t="s">
-        <v>93</v>
-      </c>
-      <c r="H64">
+      <c r="E65" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" t="s">
+        <v>97</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+      <c r="I65">
+        <v>4</v>
+      </c>
+      <c r="J65" t="s">
+        <v>147</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
+        <v>85</v>
+      </c>
+      <c r="E66" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" t="s">
+        <v>97</v>
+      </c>
+      <c r="H66">
+        <v>8</v>
+      </c>
+      <c r="I66">
+        <v>8</v>
+      </c>
+      <c r="J66" t="s">
+        <v>103</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" t="s">
+        <v>88</v>
+      </c>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67">
+        <v>4</v>
+      </c>
+      <c r="I67">
+        <v>8</v>
+      </c>
+      <c r="J67" t="s">
+        <v>148</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E68" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" t="s">
+        <v>97</v>
+      </c>
+      <c r="H68">
         <v>5</v>
       </c>
-      <c r="I64">
+      <c r="I68">
         <v>9</v>
       </c>
-      <c r="J64" t="s">
-        <v>141</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>204</v>
+      <c r="J68" t="s">
+        <v>149</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3169,6 +3333,10 @@
     <hyperlink ref="K62" r:id="rId61"/>
     <hyperlink ref="K63" r:id="rId62"/>
     <hyperlink ref="K64" r:id="rId63"/>
+    <hyperlink ref="K65" r:id="rId64"/>
+    <hyperlink ref="K66" r:id="rId65"/>
+    <hyperlink ref="K67" r:id="rId66"/>
+    <hyperlink ref="K68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>